<commit_message>
renaming picture file names
</commit_message>
<xml_diff>
--- a/Entries.xlsx
+++ b/Entries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://docs.philips.com/personal/folke_noertemann_philips_com/Documents/MyOwnStuff/WauWau/BSDS/CSC26/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{451D60E7-5808-4E94-B5F6-B6D1077C5795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8BF1E5C-C578-4A1A-A539-703CA9DA8A45}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{451D60E7-5808-4E94-B5F6-B6D1077C5795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D43975CD-489F-40A9-97BF-A940A31F9AC4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>Dog</t>
   </si>
@@ -93,21 +93,6 @@
     <t>Eryn</t>
   </si>
   <si>
-    <t>Fifi</t>
-  </si>
-  <si>
-    <t>Marie Meier</t>
-  </si>
-  <si>
-    <t>A.N. Breeder</t>
-  </si>
-  <si>
-    <t>Papa</t>
-  </si>
-  <si>
-    <t>Mama</t>
-  </si>
-  <si>
     <t>Angie Driscoll</t>
   </si>
   <si>
@@ -144,25 +129,22 @@
     <t>crazy mommy</t>
   </si>
   <si>
-    <t>PicturesOrig\FolkeNoertemannArlo.jpg</t>
-  </si>
-  <si>
-    <t>PicturesOrig\AnnieVanderlinckMoss.jpg</t>
-  </si>
-  <si>
-    <t>PicturesOrig\AnnieVanderlinckTweed.jpg</t>
-  </si>
-  <si>
-    <t>PicturesOrig\MarieMeierFifi.jpg</t>
-  </si>
-  <si>
-    <t>PicturesOrig\FolkeNoertemannKinloch Luke.jpg</t>
-  </si>
-  <si>
-    <t>PicturesOrig\FolkeNoertemannKinloch Heath.jpg</t>
-  </si>
-  <si>
-    <t>PicturesOrig\FolkeNoertemannWern Joe.jpg</t>
+    <t>PicturesOrig\FolkeNoertemann_Arlo.jpg</t>
+  </si>
+  <si>
+    <t>PicturesOrig\AnnieVanderlinck_Moss.jpg</t>
+  </si>
+  <si>
+    <t>PicturesOrig\AnnieVanderlinck_Tweed.jpg</t>
+  </si>
+  <si>
+    <t>PicturesOrig\FolkeNoertemannKinloch_Luke.jpg</t>
+  </si>
+  <si>
+    <t>PicturesOrig\FolkeNoertemannKinloch_Heath.jpg</t>
+  </si>
+  <si>
+    <t>PicturesOrig\FolkeNoertemann_Joe.jpg</t>
   </si>
 </sst>
 </file>
@@ -609,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -676,7 +658,7 @@
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -702,7 +684,7 @@
         <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -728,76 +710,76 @@
         <v>22</v>
       </c>
       <c r="H4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" s="1">
+        <v>42450</v>
+      </c>
+      <c r="E5">
+        <v>2345676</v>
+      </c>
+      <c r="F5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="1">
-        <v>42555</v>
-      </c>
-      <c r="E5">
-        <v>234777</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>26</v>
       </c>
-      <c r="G5" t="s">
-        <v>27</v>
-      </c>
       <c r="H5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1">
+        <v>43322</v>
+      </c>
+      <c r="E6">
+        <v>33333</v>
+      </c>
+      <c r="F6" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="1">
-        <v>42450</v>
-      </c>
-      <c r="E6">
-        <v>2345676</v>
-      </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
       <c r="G6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1">
-        <v>43322</v>
-      </c>
-      <c r="E7">
-        <v>33333</v>
+        <v>44247</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
       </c>
       <c r="F7" t="s">
         <v>33</v>
@@ -806,33 +788,7 @@
         <v>34</v>
       </c>
       <c r="H7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="1">
-        <v>44247</v>
-      </c>
-      <c r="E8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -866,21 +822,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<TemplafyTemplateConfiguration><![CDATA[{"transformationConfigurations":[],"templateName":"Blank workbook (1)","templateDescription":"","enableDocumentContentUpdater":false,"version":"2.0"}]]></TemplafyTemplateConfiguration>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <TemplafyFormConfiguration><![CDATA[{"formFields":[],"formDataEntries":[]}]]></TemplafyFormConfiguration>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<TemplafyTemplateConfiguration><![CDATA[{"transformationConfigurations":[],"templateName":"Blank workbook (1)","templateDescription":"","enableDocumentContentUpdater":false,"version":"2.0"}]]></TemplafyTemplateConfiguration>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D935B92B-7CB7-4F33-8A9E-9593CFA73A38}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6F80FD2-C12F-42D4-B161-EC42684C5897}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6F80FD2-C12F-42D4-B161-EC42684C5897}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D935B92B-7CB7-4F33-8A9E-9593CFA73A38}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
added the PicturesOrig dir and the files in it
</commit_message>
<xml_diff>
--- a/Entries.xlsx
+++ b/Entries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://docs.philips.com/personal/folke_noertemann_philips_com/Documents/MyOwnStuff/WauWau/BSDS/CSC26/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{451D60E7-5808-4E94-B5F6-B6D1077C5795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D43975CD-489F-40A9-97BF-A940A31F9AC4}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{451D60E7-5808-4E94-B5F6-B6D1077C5795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F2C3289-03C4-4CE2-810F-CDE0C86927A7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,22 +129,22 @@
     <t>crazy mommy</t>
   </si>
   <si>
-    <t>PicturesOrig\FolkeNoertemann_Arlo.jpg</t>
-  </si>
-  <si>
-    <t>PicturesOrig\AnnieVanderlinck_Moss.jpg</t>
-  </si>
-  <si>
-    <t>PicturesOrig\AnnieVanderlinck_Tweed.jpg</t>
-  </si>
-  <si>
-    <t>PicturesOrig\FolkeNoertemannKinloch_Luke.jpg</t>
-  </si>
-  <si>
-    <t>PicturesOrig\FolkeNoertemannKinloch_Heath.jpg</t>
-  </si>
-  <si>
-    <t>PicturesOrig\FolkeNoertemann_Joe.jpg</t>
+    <t>PicturesOrig/FolkeNoertemann_Arlo.jpg</t>
+  </si>
+  <si>
+    <t>PicturesOrig/AnnieVanderlinck_Moss.jpg</t>
+  </si>
+  <si>
+    <t>PicturesOrig/AnnieVanderlinck_Tweed.jpg</t>
+  </si>
+  <si>
+    <t>PicturesOrig/FolkeNoertemann_Joe.jpg</t>
+  </si>
+  <si>
+    <t>PicturesOrig/FolkeNoertemann_Heath.jpg</t>
+  </si>
+  <si>
+    <t>PicturesOrig/FolkeNoertemann_Luke.jpg</t>
   </si>
 </sst>
 </file>
@@ -594,7 +594,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -736,7 +736,7 @@
         <v>26</v>
       </c>
       <c r="H5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -788,7 +788,7 @@
         <v>34</v>
       </c>
       <c r="H7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaned up plus improved the automatic switching
</commit_message>
<xml_diff>
--- a/Entries.xlsx
+++ b/Entries.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://docs.philips.com/personal/folke_noertemann_philips_com/Documents/MyOwnStuff/WauWau/BSDS/CSC26/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\folke\repos\csc26_firstclone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{451D60E7-5808-4E94-B5F6-B6D1077C5795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F2C3289-03C4-4CE2-810F-CDE0C86927A7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD17578-BDCD-4EDB-B13B-0D15456ED198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
   <si>
     <t>Dog</t>
   </si>
@@ -198,10 +198,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -591,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -791,6 +787,110 @@
         <v>38</v>
       </c>
     </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1">
+        <v>39861</v>
+      </c>
+      <c r="E8">
+        <v>123435</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1">
+        <v>45433</v>
+      </c>
+      <c r="E9">
+        <v>12345</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="1">
+        <v>44247</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="1">
+        <v>43322</v>
+      </c>
+      <c r="E11">
+        <v>33333</v>
+      </c>
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>